<commit_message>
Add sample for non database
</commit_message>
<xml_diff>
--- a/src/main/resources/report/sample.xlsx
+++ b/src/main/resources/report/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/USB DISK/IdeaProjects/proto/openreports_scala/src/main/resources/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ijufumi/workspaces/ijufumi/production/openreports-api/src/main/resources/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B19AEFB-A6F6-494C-892C-08FA90577CFF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4792B109-4F03-9B41-8DF1-355153B7DE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{3C197EC1-2AF9-C04B-AB58-5E204AD8FB07}"/>
   </bookViews>
@@ -43,56 +43,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E755F418-E282-A845-AC27-D65FCF9FDA89}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">jx:each(items="jdbc.query('select * from t_member')" var="mem" lastCell="B3")
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>member_id</t>
-  </si>
-  <si>
-    <t>email_address</t>
-  </si>
-  <si>
-    <t>${mem.member_id}</t>
-  </si>
-  <si>
-    <t>${mem.email_address}</t>
+    <t>${today}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,28 +68,16 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,11 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA918369-A205-4A4F-9447-99770A7F7E72}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,25 +418,9 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>